<commit_message>
hopefully last bug fixes
</commit_message>
<xml_diff>
--- a/Notebooks/Student-Data.xlsx
+++ b/Notebooks/Student-Data.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/missd/Desktop/ML2 - Abschlussprojekt/ml2_project/Notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360FF8BA-8354-474E-98C3-E7BBC14BC0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56106D5-C4C5-2140-BD66-FB80F1464443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1280" windowWidth="28040" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="1280" windowWidth="28040" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Semester_Data" sheetId="2" r:id="rId2"/>
     <sheet name="Assessments_Data" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="89">
   <si>
     <t>diagnose</t>
   </si>
@@ -30,33 +43,15 @@
     <t>Banner</t>
   </si>
   <si>
-    <t>Barton</t>
-  </si>
-  <si>
     <t>Romanoff</t>
   </si>
   <si>
-    <t>Rogers</t>
-  </si>
-  <si>
-    <t>Stark</t>
-  </si>
-  <si>
     <t>Bruce</t>
   </si>
   <si>
-    <t>Clint</t>
-  </si>
-  <si>
     <t>Natasha</t>
   </si>
   <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>Tony</t>
-  </si>
-  <si>
     <t>männlich</t>
   </si>
   <si>
@@ -66,30 +61,15 @@
     <t>Schizophrenie</t>
   </si>
   <si>
-    <t>Autismus-Spektrums-Störung</t>
-  </si>
-  <si>
-    <t>Narzistische Persönlichkeitsstörung</t>
-  </si>
-  <si>
     <t>2009-02-02</t>
   </si>
   <si>
-    <t>2009-04-04</t>
-  </si>
-  <si>
     <t>2009-03-03</t>
   </si>
   <si>
-    <t>2009-01-01</t>
-  </si>
-  <si>
     <t>2022-08-01</t>
   </si>
   <si>
-    <t>2020-08-01</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -99,9 +79,6 @@
     <t>Separater Raum bei Prüfungen</t>
   </si>
   <si>
-    <t>Separater Raum bei Prüfungen, mehr Zeit bei Prüfungen</t>
-  </si>
-  <si>
     <t>Miss Marvel</t>
   </si>
   <si>
@@ -117,9 +94,6 @@
     <t>FS23</t>
   </si>
   <si>
-    <t>FS22</t>
-  </si>
-  <si>
     <t>AktivTeilnehmenNotizen</t>
   </si>
   <si>
@@ -135,12 +109,6 @@
     <t>SchulinhalteAbrufenNotizen</t>
   </si>
   <si>
-    <t>2024-06-01T09:42:13.695+00:00</t>
-  </si>
-  <si>
-    <t>Daniela</t>
-  </si>
-  <si>
     <t>AktivTeilnehmen</t>
   </si>
   <si>
@@ -174,9 +142,6 @@
     <t>ab und zu fällt es Bruce schwer, bei Prüfungen zu zeigen, was er kann.</t>
   </si>
   <si>
-    <t>Yves</t>
-  </si>
-  <si>
     <t>noch nicht</t>
   </si>
   <si>
@@ -186,9 +151,6 @@
     <t>Bruce hat viele schulische Interessen. Insbesondere in Physik und Chemie ist er sehr gut</t>
   </si>
   <si>
-    <t>Bruce hat sich seit dem letzten Semester sehr verbessert</t>
-  </si>
-  <si>
     <t>lastname</t>
   </si>
   <si>
@@ -225,19 +187,121 @@
     <t>date</t>
   </si>
   <si>
-    <t>2023-06-01T09:42:14.695+00:00</t>
-  </si>
-  <si>
     <t>2023-06-01T09:42:13.695+00:00</t>
   </si>
   <si>
-    <t>2024-06-01T09:42:14.695+00:00</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
     <t>semester_name</t>
+  </si>
+  <si>
+    <t>Teacher1</t>
+  </si>
+  <si>
+    <t>Teacher2</t>
+  </si>
+  <si>
+    <t>Teacher3</t>
+  </si>
+  <si>
+    <t>Natasha ist besonders beim Sport aktiv dabei</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:42:14.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:43:13.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:44:13.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:45:14.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:46:13.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-06-01T09:43:14.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-06-01T09:49:14.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-06-01T09:48:14.695+00:00</t>
+  </si>
+  <si>
+    <t>2023-06-01T09:47:13.695+00:00</t>
+  </si>
+  <si>
+    <t>Bruce ist meistens aktiv in der Schule</t>
+  </si>
+  <si>
+    <t>Oft ist er im Unterricht aufmerksam.</t>
+  </si>
+  <si>
+    <t>Es kann vorkommen, dass er etwas verträumt ist.</t>
+  </si>
+  <si>
+    <t>nicht immer</t>
+  </si>
+  <si>
+    <t>er vegisst nach den Prüfungen vieles</t>
+  </si>
+  <si>
+    <t>teilweise ist er sehr müde</t>
+  </si>
+  <si>
+    <t>er meldet sich oft im Unterricht</t>
+  </si>
+  <si>
+    <t>wenn er nicht müde ist, geht es gut</t>
+  </si>
+  <si>
+    <t>Sport ist ihr bestes Fach, aber sie ist auch gut in Sprachen</t>
+  </si>
+  <si>
+    <t>sie zeigt immer super Leistungen</t>
+  </si>
+  <si>
+    <t>ihre Leistungen sind meistens super</t>
+  </si>
+  <si>
+    <t>bei Themen, die ihn interessieren, kann er sich sehr viel merken, sonst ist es schwierig</t>
+  </si>
+  <si>
+    <t>sie kann sich die Prüfungsinhalte gut merken</t>
+  </si>
+  <si>
+    <t>wenn sie ein Fach nicht interessiert, geht es nicht so gut</t>
+  </si>
+  <si>
+    <t>ab und zu fällt es Natasha schwer, bei Prüfungen zu zeigen, was sie kann.</t>
+  </si>
+  <si>
+    <t>manchmal hat sie Schwierigkeiten, bei Prüfungen zu zeigen, was sie kann.</t>
+  </si>
+  <si>
+    <t>grade_level</t>
+  </si>
+  <si>
+    <t>1. Sekundarstufe</t>
+  </si>
+  <si>
+    <t>3. Sekundarstufe</t>
+  </si>
+  <si>
+    <t>2. Sekundarstufe</t>
+  </si>
+  <si>
+    <t>6. Klasse</t>
+  </si>
+  <si>
+    <t>HS22</t>
+  </si>
+  <si>
+    <t>keines</t>
   </si>
 </sst>
 </file>
@@ -246,7 +310,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -590,7 +654,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -705,6 +769,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -750,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -762,13 +906,40 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1124,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,167 +1315,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>70</v>
+      <c r="A1" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>62</v>
+      <c r="G1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1314,292 +1404,160 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D806464F-D998-BD46-8CF9-01451E50C39F}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="3" width="11.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>64</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>29</v>
+        <v>87</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>31</v>
+        <v>87</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1610,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A45F847-6263-6742-BA38-81A6A0D0B402}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1623,188 +1581,428 @@
     <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="102" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>67</v>
+      <c r="E2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
+      <c r="A3" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="7" t="s">
+    </row>
+    <row r="6" spans="1:14" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>68</v>
+      <c r="D7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="7" t="s">
+    <row r="8" spans="1:14" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="8" t="s">
-        <v>37</v>
+      <c r="D8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="8" t="s">
-        <v>69</v>
+    <row r="9" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>